<commit_message>
Changed sample documents (karakulina)
git-svn-id: https://svn.l3s.uni-hannover.de/learnweb/trunk/LearnwebOER/Learnweb@5496 422a2c9f-66af-4668-9993-60dc3b0871b8
</commit_message>
<xml_diff>
--- a/Resources/de/l3s/learnweb/office/documents/sample.xlsx
+++ b/Resources/de/l3s/learnweb/office/documents/sample.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -32,7 +27,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
@@ -45,23 +40,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -99,18 +94,18 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -138,13 +133,13 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -169,7 +164,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,43 +336,224 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>